<commit_message>
final changes of browser size
</commit_message>
<xml_diff>
--- a/FedExCIL/TestFiles/FedExCILTestResult.xlsx
+++ b/FedExCIL/TestFiles/FedExCILTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>FileName</t>
   </si>
@@ -107,6 +107,306 @@
   </si>
   <si>
     <t>32265028</t>
+  </si>
+  <si>
+    <t>32288437</t>
+  </si>
+  <si>
+    <t>32288438</t>
+  </si>
+  <si>
+    <t>32288439</t>
+  </si>
+  <si>
+    <t>32288440</t>
+  </si>
+  <si>
+    <t>32288441</t>
+  </si>
+  <si>
+    <t>32288442</t>
+  </si>
+  <si>
+    <t>32288443</t>
+  </si>
+  <si>
+    <t>32288444</t>
+  </si>
+  <si>
+    <t>32288445</t>
+  </si>
+  <si>
+    <t>32288446</t>
+  </si>
+  <si>
+    <t>32288448</t>
+  </si>
+  <si>
+    <t>32288449</t>
+  </si>
+  <si>
+    <t>32288451</t>
+  </si>
+  <si>
+    <t>32288452</t>
+  </si>
+  <si>
+    <t>32288453</t>
+  </si>
+  <si>
+    <t>32288454</t>
+  </si>
+  <si>
+    <t>32288455</t>
+  </si>
+  <si>
+    <t>32288456</t>
+  </si>
+  <si>
+    <t>32288457</t>
+  </si>
+  <si>
+    <t>32288458</t>
+  </si>
+  <si>
+    <t>32288459</t>
+  </si>
+  <si>
+    <t>32288460</t>
+  </si>
+  <si>
+    <t>32288461</t>
+  </si>
+  <si>
+    <t>32288462</t>
+  </si>
+  <si>
+    <t>32288463</t>
+  </si>
+  <si>
+    <t>32288464</t>
+  </si>
+  <si>
+    <t>32288466</t>
+  </si>
+  <si>
+    <t>32288468</t>
+  </si>
+  <si>
+    <t>32288469</t>
+  </si>
+  <si>
+    <t>32288470</t>
+  </si>
+  <si>
+    <t>32288477</t>
+  </si>
+  <si>
+    <t>32288478</t>
+  </si>
+  <si>
+    <t>32288479</t>
+  </si>
+  <si>
+    <t>32288480</t>
+  </si>
+  <si>
+    <t>32288481</t>
+  </si>
+  <si>
+    <t>32288482</t>
+  </si>
+  <si>
+    <t>32288483</t>
+  </si>
+  <si>
+    <t>32288484</t>
+  </si>
+  <si>
+    <t>32288485</t>
+  </si>
+  <si>
+    <t>32288486</t>
+  </si>
+  <si>
+    <t>32291133</t>
+  </si>
+  <si>
+    <t>32291134</t>
+  </si>
+  <si>
+    <t>32291135</t>
+  </si>
+  <si>
+    <t>32291136</t>
+  </si>
+  <si>
+    <t>32291137</t>
+  </si>
+  <si>
+    <t>32291138</t>
+  </si>
+  <si>
+    <t>32291139</t>
+  </si>
+  <si>
+    <t>32291140</t>
+  </si>
+  <si>
+    <t>32291141</t>
+  </si>
+  <si>
+    <t>32291142</t>
+  </si>
+  <si>
+    <t>32291143</t>
+  </si>
+  <si>
+    <t>32291144</t>
+  </si>
+  <si>
+    <t>32291145</t>
+  </si>
+  <si>
+    <t>32291146</t>
+  </si>
+  <si>
+    <t>32291147</t>
+  </si>
+  <si>
+    <t>32291148</t>
+  </si>
+  <si>
+    <t>32291149</t>
+  </si>
+  <si>
+    <t>32291150</t>
+  </si>
+  <si>
+    <t>32291151</t>
+  </si>
+  <si>
+    <t>32291152</t>
+  </si>
+  <si>
+    <t>32291162</t>
+  </si>
+  <si>
+    <t>32291163</t>
+  </si>
+  <si>
+    <t>32291164</t>
+  </si>
+  <si>
+    <t>32291165</t>
+  </si>
+  <si>
+    <t>32291166</t>
+  </si>
+  <si>
+    <t>32291167</t>
+  </si>
+  <si>
+    <t>32291168</t>
+  </si>
+  <si>
+    <t>32291169</t>
+  </si>
+  <si>
+    <t>32291170</t>
+  </si>
+  <si>
+    <t>32291171</t>
+  </si>
+  <si>
+    <t>32294100</t>
+  </si>
+  <si>
+    <t>32294101</t>
+  </si>
+  <si>
+    <t>32294102</t>
+  </si>
+  <si>
+    <t>32294103</t>
+  </si>
+  <si>
+    <t>32294104</t>
+  </si>
+  <si>
+    <t>32294105</t>
+  </si>
+  <si>
+    <t>32294107</t>
+  </si>
+  <si>
+    <t>32294108</t>
+  </si>
+  <si>
+    <t>32294109</t>
+  </si>
+  <si>
+    <t>32294111</t>
+  </si>
+  <si>
+    <t>32296080</t>
+  </si>
+  <si>
+    <t>32296081</t>
+  </si>
+  <si>
+    <t>32296082</t>
+  </si>
+  <si>
+    <t>32296083</t>
+  </si>
+  <si>
+    <t>32296084</t>
+  </si>
+  <si>
+    <t>32296085</t>
+  </si>
+  <si>
+    <t>32296086</t>
+  </si>
+  <si>
+    <t>32296087</t>
+  </si>
+  <si>
+    <t>32296088</t>
+  </si>
+  <si>
+    <t>32296089</t>
+  </si>
+  <si>
+    <t>32297175</t>
+  </si>
+  <si>
+    <t>32297176</t>
+  </si>
+  <si>
+    <t>32297178</t>
+  </si>
+  <si>
+    <t>32297180</t>
+  </si>
+  <si>
+    <t>32297186</t>
+  </si>
+  <si>
+    <t>32297193</t>
+  </si>
+  <si>
+    <t>32297201</t>
+  </si>
+  <si>
+    <t>32297209</t>
+  </si>
+  <si>
+    <t>32297242</t>
+  </si>
+  <si>
+    <t>32297272</t>
   </si>
 </sst>
 </file>
@@ -459,7 +759,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -484,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -492,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -500,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -508,7 +808,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -516,7 +816,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -524,7 +824,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -532,7 +832,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -540,7 +840,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -548,7 +848,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -556,7 +856,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>

<commit_message>
Changes of 1st Apr 2022
</commit_message>
<xml_diff>
--- a/FedExCIL/TestFiles/FedExCILTestResult.xlsx
+++ b/FedExCIL/TestFiles/FedExCILTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="244">
   <si>
     <t>FileName</t>
   </si>
@@ -407,6 +407,345 @@
   </si>
   <si>
     <t>32297272</t>
+  </si>
+  <si>
+    <t>32297471</t>
+  </si>
+  <si>
+    <t>32297472</t>
+  </si>
+  <si>
+    <t>32297473</t>
+  </si>
+  <si>
+    <t>32297474</t>
+  </si>
+  <si>
+    <t>32297475</t>
+  </si>
+  <si>
+    <t>32297478</t>
+  </si>
+  <si>
+    <t>32297481</t>
+  </si>
+  <si>
+    <t>32297482</t>
+  </si>
+  <si>
+    <t>32297483</t>
+  </si>
+  <si>
+    <t>32297484</t>
+  </si>
+  <si>
+    <t>19663449</t>
+  </si>
+  <si>
+    <t>19663458</t>
+  </si>
+  <si>
+    <t>19663460</t>
+  </si>
+  <si>
+    <t>19663511</t>
+  </si>
+  <si>
+    <t>19663362</t>
+  </si>
+  <si>
+    <t>19667650</t>
+  </si>
+  <si>
+    <t>19667611</t>
+  </si>
+  <si>
+    <t>19667593</t>
+  </si>
+  <si>
+    <t>19667541</t>
+  </si>
+  <si>
+    <t>19667542</t>
+  </si>
+  <si>
+    <t>32304492</t>
+  </si>
+  <si>
+    <t>32304493</t>
+  </si>
+  <si>
+    <t>32304494</t>
+  </si>
+  <si>
+    <t>32304495</t>
+  </si>
+  <si>
+    <t>32304496</t>
+  </si>
+  <si>
+    <t>32304497</t>
+  </si>
+  <si>
+    <t>32304498</t>
+  </si>
+  <si>
+    <t>32304499</t>
+  </si>
+  <si>
+    <t>32304500</t>
+  </si>
+  <si>
+    <t>32304501</t>
+  </si>
+  <si>
+    <t>32305720</t>
+  </si>
+  <si>
+    <t>32305721</t>
+  </si>
+  <si>
+    <t>32305722</t>
+  </si>
+  <si>
+    <t>32305723</t>
+  </si>
+  <si>
+    <t>32305724</t>
+  </si>
+  <si>
+    <t>32305726</t>
+  </si>
+  <si>
+    <t>32305727</t>
+  </si>
+  <si>
+    <t>32305728</t>
+  </si>
+  <si>
+    <t>32305729</t>
+  </si>
+  <si>
+    <t>32306383</t>
+  </si>
+  <si>
+    <t>32306384</t>
+  </si>
+  <si>
+    <t>32306386</t>
+  </si>
+  <si>
+    <t>32306387</t>
+  </si>
+  <si>
+    <t>32306388</t>
+  </si>
+  <si>
+    <t>32306389</t>
+  </si>
+  <si>
+    <t>32306390</t>
+  </si>
+  <si>
+    <t>32306391</t>
+  </si>
+  <si>
+    <t>32306392</t>
+  </si>
+  <si>
+    <t>32306393</t>
+  </si>
+  <si>
+    <t>32310095</t>
+  </si>
+  <si>
+    <t>32310096</t>
+  </si>
+  <si>
+    <t>32310097</t>
+  </si>
+  <si>
+    <t>32310099</t>
+  </si>
+  <si>
+    <t>32310100</t>
+  </si>
+  <si>
+    <t>32310101</t>
+  </si>
+  <si>
+    <t>32312653</t>
+  </si>
+  <si>
+    <t>32312654</t>
+  </si>
+  <si>
+    <t>32312655</t>
+  </si>
+  <si>
+    <t>32312656</t>
+  </si>
+  <si>
+    <t>32312657</t>
+  </si>
+  <si>
+    <t>32312658</t>
+  </si>
+  <si>
+    <t>32312659</t>
+  </si>
+  <si>
+    <t>32312660</t>
+  </si>
+  <si>
+    <t>32312661</t>
+  </si>
+  <si>
+    <t>32312662</t>
+  </si>
+  <si>
+    <t>32316063</t>
+  </si>
+  <si>
+    <t>32316065</t>
+  </si>
+  <si>
+    <t>32316066</t>
+  </si>
+  <si>
+    <t>32316067</t>
+  </si>
+  <si>
+    <t>32316068</t>
+  </si>
+  <si>
+    <t>32316069</t>
+  </si>
+  <si>
+    <t>32316070</t>
+  </si>
+  <si>
+    <t>32316071</t>
+  </si>
+  <si>
+    <t>32316072</t>
+  </si>
+  <si>
+    <t>32316073</t>
+  </si>
+  <si>
+    <t>32318592</t>
+  </si>
+  <si>
+    <t>32318594</t>
+  </si>
+  <si>
+    <t>32318595</t>
+  </si>
+  <si>
+    <t>32318596</t>
+  </si>
+  <si>
+    <t>32318597</t>
+  </si>
+  <si>
+    <t>32318598</t>
+  </si>
+  <si>
+    <t>32318599</t>
+  </si>
+  <si>
+    <t>32318600</t>
+  </si>
+  <si>
+    <t>32318601</t>
+  </si>
+  <si>
+    <t>32318602</t>
+  </si>
+  <si>
+    <t>32321139</t>
+  </si>
+  <si>
+    <t>32321140</t>
+  </si>
+  <si>
+    <t>32321141</t>
+  </si>
+  <si>
+    <t>32321142</t>
+  </si>
+  <si>
+    <t>32321143</t>
+  </si>
+  <si>
+    <t>32321144</t>
+  </si>
+  <si>
+    <t>32321145</t>
+  </si>
+  <si>
+    <t>32321146</t>
+  </si>
+  <si>
+    <t>32321147</t>
+  </si>
+  <si>
+    <t>32321148</t>
+  </si>
+  <si>
+    <t>32322962</t>
+  </si>
+  <si>
+    <t>32322963</t>
+  </si>
+  <si>
+    <t>32322964</t>
+  </si>
+  <si>
+    <t>32322965</t>
+  </si>
+  <si>
+    <t>32322966</t>
+  </si>
+  <si>
+    <t>32322967</t>
+  </si>
+  <si>
+    <t>32322970</t>
+  </si>
+  <si>
+    <t>32322971</t>
+  </si>
+  <si>
+    <t>32323069</t>
+  </si>
+  <si>
+    <t>32323070</t>
+  </si>
+  <si>
+    <t>32323071</t>
+  </si>
+  <si>
+    <t>32323072</t>
+  </si>
+  <si>
+    <t>32323073</t>
+  </si>
+  <si>
+    <t>32323074</t>
+  </si>
+  <si>
+    <t>32323075</t>
+  </si>
+  <si>
+    <t>32323076</t>
+  </si>
+  <si>
+    <t>32323077</t>
+  </si>
+  <si>
+    <t>32323078</t>
   </si>
 </sst>
 </file>
@@ -759,7 +1098,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -784,7 +1123,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -792,7 +1131,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -800,7 +1139,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -808,7 +1147,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -816,7 +1155,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -824,7 +1163,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -832,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -840,7 +1179,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -848,7 +1187,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -856,7 +1195,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>

<commit_message>
Changes of OrderCreation Time
</commit_message>
<xml_diff>
--- a/FedExCIL/TestFiles/FedExCILTestResult.xlsx
+++ b/FedExCIL/TestFiles/FedExCILTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="444">
   <si>
     <t>FileName</t>
   </si>
@@ -746,6 +746,606 @@
   </si>
   <si>
     <t>32323078</t>
+  </si>
+  <si>
+    <t>32326574</t>
+  </si>
+  <si>
+    <t>32326575</t>
+  </si>
+  <si>
+    <t>32326576</t>
+  </si>
+  <si>
+    <t>32326577</t>
+  </si>
+  <si>
+    <t>32326578</t>
+  </si>
+  <si>
+    <t>32326579</t>
+  </si>
+  <si>
+    <t>32326580</t>
+  </si>
+  <si>
+    <t>32326581</t>
+  </si>
+  <si>
+    <t>32326582</t>
+  </si>
+  <si>
+    <t>32326583</t>
+  </si>
+  <si>
+    <t>32328713</t>
+  </si>
+  <si>
+    <t>32328715</t>
+  </si>
+  <si>
+    <t>32328716</t>
+  </si>
+  <si>
+    <t>32328717</t>
+  </si>
+  <si>
+    <t>32328718</t>
+  </si>
+  <si>
+    <t>32328719</t>
+  </si>
+  <si>
+    <t>32328720</t>
+  </si>
+  <si>
+    <t>32328721</t>
+  </si>
+  <si>
+    <t>32328722</t>
+  </si>
+  <si>
+    <t>32328723</t>
+  </si>
+  <si>
+    <t>32331005</t>
+  </si>
+  <si>
+    <t>32331022</t>
+  </si>
+  <si>
+    <t>32331031</t>
+  </si>
+  <si>
+    <t>32331032</t>
+  </si>
+  <si>
+    <t>32331033</t>
+  </si>
+  <si>
+    <t>32331034</t>
+  </si>
+  <si>
+    <t>32331035</t>
+  </si>
+  <si>
+    <t>32331036</t>
+  </si>
+  <si>
+    <t>32331037</t>
+  </si>
+  <si>
+    <t>32331038</t>
+  </si>
+  <si>
+    <t>32333900</t>
+  </si>
+  <si>
+    <t>32333901</t>
+  </si>
+  <si>
+    <t>32333902</t>
+  </si>
+  <si>
+    <t>32333903</t>
+  </si>
+  <si>
+    <t>32333904</t>
+  </si>
+  <si>
+    <t>32333905</t>
+  </si>
+  <si>
+    <t>32333913</t>
+  </si>
+  <si>
+    <t>32333914</t>
+  </si>
+  <si>
+    <t>32333916</t>
+  </si>
+  <si>
+    <t>32333923</t>
+  </si>
+  <si>
+    <t>32336059</t>
+  </si>
+  <si>
+    <t>32336060</t>
+  </si>
+  <si>
+    <t>32336061</t>
+  </si>
+  <si>
+    <t>32336064</t>
+  </si>
+  <si>
+    <t>32336065</t>
+  </si>
+  <si>
+    <t>32336066</t>
+  </si>
+  <si>
+    <t>32336067</t>
+  </si>
+  <si>
+    <t>32336068</t>
+  </si>
+  <si>
+    <t>32336069</t>
+  </si>
+  <si>
+    <t>32336070</t>
+  </si>
+  <si>
+    <t>32339596</t>
+  </si>
+  <si>
+    <t>32339604</t>
+  </si>
+  <si>
+    <t>32339605</t>
+  </si>
+  <si>
+    <t>32339613</t>
+  </si>
+  <si>
+    <t>32339615</t>
+  </si>
+  <si>
+    <t>32339623</t>
+  </si>
+  <si>
+    <t>32339637</t>
+  </si>
+  <si>
+    <t>32339656</t>
+  </si>
+  <si>
+    <t>32339669</t>
+  </si>
+  <si>
+    <t>32339682</t>
+  </si>
+  <si>
+    <t>32341463</t>
+  </si>
+  <si>
+    <t>32341464</t>
+  </si>
+  <si>
+    <t>32341465</t>
+  </si>
+  <si>
+    <t>32341466</t>
+  </si>
+  <si>
+    <t>32341467</t>
+  </si>
+  <si>
+    <t>32341468</t>
+  </si>
+  <si>
+    <t>32341470</t>
+  </si>
+  <si>
+    <t>32341471</t>
+  </si>
+  <si>
+    <t>32341472</t>
+  </si>
+  <si>
+    <t>32341473</t>
+  </si>
+  <si>
+    <t>32343360</t>
+  </si>
+  <si>
+    <t>32343361</t>
+  </si>
+  <si>
+    <t>32343362</t>
+  </si>
+  <si>
+    <t>32343363</t>
+  </si>
+  <si>
+    <t>32343364</t>
+  </si>
+  <si>
+    <t>32343365</t>
+  </si>
+  <si>
+    <t>32343366</t>
+  </si>
+  <si>
+    <t>32343367</t>
+  </si>
+  <si>
+    <t>32343368</t>
+  </si>
+  <si>
+    <t>32343369</t>
+  </si>
+  <si>
+    <t>32345337</t>
+  </si>
+  <si>
+    <t>32345338</t>
+  </si>
+  <si>
+    <t>32345339</t>
+  </si>
+  <si>
+    <t>32345340</t>
+  </si>
+  <si>
+    <t>32345341</t>
+  </si>
+  <si>
+    <t>32345342</t>
+  </si>
+  <si>
+    <t>32345354</t>
+  </si>
+  <si>
+    <t>32345355</t>
+  </si>
+  <si>
+    <t>32345356</t>
+  </si>
+  <si>
+    <t>32345357</t>
+  </si>
+  <si>
+    <t>32346980</t>
+  </si>
+  <si>
+    <t>32346981</t>
+  </si>
+  <si>
+    <t>32346982</t>
+  </si>
+  <si>
+    <t>32346983</t>
+  </si>
+  <si>
+    <t>32346984</t>
+  </si>
+  <si>
+    <t>32346985</t>
+  </si>
+  <si>
+    <t>32346986</t>
+  </si>
+  <si>
+    <t>32346987</t>
+  </si>
+  <si>
+    <t>32346988</t>
+  </si>
+  <si>
+    <t>32346989</t>
+  </si>
+  <si>
+    <t>32350078</t>
+  </si>
+  <si>
+    <t>32350093</t>
+  </si>
+  <si>
+    <t>32350106</t>
+  </si>
+  <si>
+    <t>32350107</t>
+  </si>
+  <si>
+    <t>32350108</t>
+  </si>
+  <si>
+    <t>32350109</t>
+  </si>
+  <si>
+    <t>32350110</t>
+  </si>
+  <si>
+    <t>32350111</t>
+  </si>
+  <si>
+    <t>32350112</t>
+  </si>
+  <si>
+    <t>32350113</t>
+  </si>
+  <si>
+    <t>32351999</t>
+  </si>
+  <si>
+    <t>32352007</t>
+  </si>
+  <si>
+    <t>32352014</t>
+  </si>
+  <si>
+    <t>32352021</t>
+  </si>
+  <si>
+    <t>32352028</t>
+  </si>
+  <si>
+    <t>32352041</t>
+  </si>
+  <si>
+    <t>32352056</t>
+  </si>
+  <si>
+    <t>32352069</t>
+  </si>
+  <si>
+    <t>32352084</t>
+  </si>
+  <si>
+    <t>32352101</t>
+  </si>
+  <si>
+    <t>32356487</t>
+  </si>
+  <si>
+    <t>32356488</t>
+  </si>
+  <si>
+    <t>32356489</t>
+  </si>
+  <si>
+    <t>32356490</t>
+  </si>
+  <si>
+    <t>32356491</t>
+  </si>
+  <si>
+    <t>32356492</t>
+  </si>
+  <si>
+    <t>32356493</t>
+  </si>
+  <si>
+    <t>32356494</t>
+  </si>
+  <si>
+    <t>32356495</t>
+  </si>
+  <si>
+    <t>32356497</t>
+  </si>
+  <si>
+    <t>32358979</t>
+  </si>
+  <si>
+    <t>32358981</t>
+  </si>
+  <si>
+    <t>32358987</t>
+  </si>
+  <si>
+    <t>32358995</t>
+  </si>
+  <si>
+    <t>32359010</t>
+  </si>
+  <si>
+    <t>32359023</t>
+  </si>
+  <si>
+    <t>32359036</t>
+  </si>
+  <si>
+    <t>32359045</t>
+  </si>
+  <si>
+    <t>32359062</t>
+  </si>
+  <si>
+    <t>32359073</t>
+  </si>
+  <si>
+    <t>32363565</t>
+  </si>
+  <si>
+    <t>32363569</t>
+  </si>
+  <si>
+    <t>32363570</t>
+  </si>
+  <si>
+    <t>32363571</t>
+  </si>
+  <si>
+    <t>32363572</t>
+  </si>
+  <si>
+    <t>32363573</t>
+  </si>
+  <si>
+    <t>32363574</t>
+  </si>
+  <si>
+    <t>32363575</t>
+  </si>
+  <si>
+    <t>32363576</t>
+  </si>
+  <si>
+    <t>32363577</t>
+  </si>
+  <si>
+    <t>32367098</t>
+  </si>
+  <si>
+    <t>32367099</t>
+  </si>
+  <si>
+    <t>32367100</t>
+  </si>
+  <si>
+    <t>32367101</t>
+  </si>
+  <si>
+    <t>32367102</t>
+  </si>
+  <si>
+    <t>32367103</t>
+  </si>
+  <si>
+    <t>32367104</t>
+  </si>
+  <si>
+    <t>32367105</t>
+  </si>
+  <si>
+    <t>32367106</t>
+  </si>
+  <si>
+    <t>32367107</t>
+  </si>
+  <si>
+    <t>32369419</t>
+  </si>
+  <si>
+    <t>32369437</t>
+  </si>
+  <si>
+    <t>32369438</t>
+  </si>
+  <si>
+    <t>32369446</t>
+  </si>
+  <si>
+    <t>32369454</t>
+  </si>
+  <si>
+    <t>32369455</t>
+  </si>
+  <si>
+    <t>32369460</t>
+  </si>
+  <si>
+    <t>32369471</t>
+  </si>
+  <si>
+    <t>32369490</t>
+  </si>
+  <si>
+    <t>32369503</t>
+  </si>
+  <si>
+    <t>32371761</t>
+  </si>
+  <si>
+    <t>32371762</t>
+  </si>
+  <si>
+    <t>32371763</t>
+  </si>
+  <si>
+    <t>32371764</t>
+  </si>
+  <si>
+    <t>32371772</t>
+  </si>
+  <si>
+    <t>32371774</t>
+  </si>
+  <si>
+    <t>32371782</t>
+  </si>
+  <si>
+    <t>32371783</t>
+  </si>
+  <si>
+    <t>32371790</t>
+  </si>
+  <si>
+    <t>32371791</t>
+  </si>
+  <si>
+    <t>32374011</t>
+  </si>
+  <si>
+    <t>32374016</t>
+  </si>
+  <si>
+    <t>32374023</t>
+  </si>
+  <si>
+    <t>32374036</t>
+  </si>
+  <si>
+    <t>32374049</t>
+  </si>
+  <si>
+    <t>32374058</t>
+  </si>
+  <si>
+    <t>32374071</t>
+  </si>
+  <si>
+    <t>32374084</t>
+  </si>
+  <si>
+    <t>32374099</t>
+  </si>
+  <si>
+    <t>32374108</t>
+  </si>
+  <si>
+    <t>32376236</t>
+  </si>
+  <si>
+    <t>32376237</t>
+  </si>
+  <si>
+    <t>32376238</t>
+  </si>
+  <si>
+    <t>32376239</t>
+  </si>
+  <si>
+    <t>32376241</t>
+  </si>
+  <si>
+    <t>32376242</t>
+  </si>
+  <si>
+    <t>32376243</t>
+  </si>
+  <si>
+    <t>32376244</t>
+  </si>
+  <si>
+    <t>32376245</t>
+  </si>
+  <si>
+    <t>32376246</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1698,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -1123,7 +1723,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1131,7 +1731,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1139,7 +1739,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>236</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1147,7 +1747,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>237</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1155,7 +1755,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1163,7 +1763,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1171,7 +1771,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>240</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1179,7 +1779,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1187,7 +1787,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>242</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1195,7 +1795,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>243</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>

<commit_message>
Changes of Config file
</commit_message>
<xml_diff>
--- a/FedExCIL/TestFiles/FedExCILTestResult.xlsx
+++ b/FedExCIL/TestFiles/FedExCILTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="574">
   <si>
     <t>FileName</t>
   </si>
@@ -1346,6 +1346,396 @@
   </si>
   <si>
     <t>32376246</t>
+  </si>
+  <si>
+    <t>32376664</t>
+  </si>
+  <si>
+    <t>32376665</t>
+  </si>
+  <si>
+    <t>32376666</t>
+  </si>
+  <si>
+    <t>32376667</t>
+  </si>
+  <si>
+    <t>32376668</t>
+  </si>
+  <si>
+    <t>32376669</t>
+  </si>
+  <si>
+    <t>32376670</t>
+  </si>
+  <si>
+    <t>32376672</t>
+  </si>
+  <si>
+    <t>32376673</t>
+  </si>
+  <si>
+    <t>32376674</t>
+  </si>
+  <si>
+    <t>32378716</t>
+  </si>
+  <si>
+    <t>32378717</t>
+  </si>
+  <si>
+    <t>32378718</t>
+  </si>
+  <si>
+    <t>32378719</t>
+  </si>
+  <si>
+    <t>32378720</t>
+  </si>
+  <si>
+    <t>32378721</t>
+  </si>
+  <si>
+    <t>32378722</t>
+  </si>
+  <si>
+    <t>32378723</t>
+  </si>
+  <si>
+    <t>32378724</t>
+  </si>
+  <si>
+    <t>32378725</t>
+  </si>
+  <si>
+    <t>32379642</t>
+  </si>
+  <si>
+    <t>32379643</t>
+  </si>
+  <si>
+    <t>32379644</t>
+  </si>
+  <si>
+    <t>32379645</t>
+  </si>
+  <si>
+    <t>32379646</t>
+  </si>
+  <si>
+    <t>32379647</t>
+  </si>
+  <si>
+    <t>32379648</t>
+  </si>
+  <si>
+    <t>32379649</t>
+  </si>
+  <si>
+    <t>32379650</t>
+  </si>
+  <si>
+    <t>32379651</t>
+  </si>
+  <si>
+    <t>32381572</t>
+  </si>
+  <si>
+    <t>32381573</t>
+  </si>
+  <si>
+    <t>32381574</t>
+  </si>
+  <si>
+    <t>32381575</t>
+  </si>
+  <si>
+    <t>32381576</t>
+  </si>
+  <si>
+    <t>32381580</t>
+  </si>
+  <si>
+    <t>32381581</t>
+  </si>
+  <si>
+    <t>32381582</t>
+  </si>
+  <si>
+    <t>32381583</t>
+  </si>
+  <si>
+    <t>32381584</t>
+  </si>
+  <si>
+    <t>32383151</t>
+  </si>
+  <si>
+    <t>32383152</t>
+  </si>
+  <si>
+    <t>32383153</t>
+  </si>
+  <si>
+    <t>32383156</t>
+  </si>
+  <si>
+    <t>32383157</t>
+  </si>
+  <si>
+    <t>32383158</t>
+  </si>
+  <si>
+    <t>32383159</t>
+  </si>
+  <si>
+    <t>32383160</t>
+  </si>
+  <si>
+    <t>32383161</t>
+  </si>
+  <si>
+    <t>32383162</t>
+  </si>
+  <si>
+    <t>32385663</t>
+  </si>
+  <si>
+    <t>32385664</t>
+  </si>
+  <si>
+    <t>32385665</t>
+  </si>
+  <si>
+    <t>32385666</t>
+  </si>
+  <si>
+    <t>32385667</t>
+  </si>
+  <si>
+    <t>32385668</t>
+  </si>
+  <si>
+    <t>32385669</t>
+  </si>
+  <si>
+    <t>32385670</t>
+  </si>
+  <si>
+    <t>32385671</t>
+  </si>
+  <si>
+    <t>32385672</t>
+  </si>
+  <si>
+    <t>32388992</t>
+  </si>
+  <si>
+    <t>32388993</t>
+  </si>
+  <si>
+    <t>32388994</t>
+  </si>
+  <si>
+    <t>32388995</t>
+  </si>
+  <si>
+    <t>32388996</t>
+  </si>
+  <si>
+    <t>32388997</t>
+  </si>
+  <si>
+    <t>32388998</t>
+  </si>
+  <si>
+    <t>32388999</t>
+  </si>
+  <si>
+    <t>32389000</t>
+  </si>
+  <si>
+    <t>32389001</t>
+  </si>
+  <si>
+    <t>32391730</t>
+  </si>
+  <si>
+    <t>32391734</t>
+  </si>
+  <si>
+    <t>32391739</t>
+  </si>
+  <si>
+    <t>32391740</t>
+  </si>
+  <si>
+    <t>32391741</t>
+  </si>
+  <si>
+    <t>32391742</t>
+  </si>
+  <si>
+    <t>32391743</t>
+  </si>
+  <si>
+    <t>32391744</t>
+  </si>
+  <si>
+    <t>32391745</t>
+  </si>
+  <si>
+    <t>32391746</t>
+  </si>
+  <si>
+    <t>32393749</t>
+  </si>
+  <si>
+    <t>32393750</t>
+  </si>
+  <si>
+    <t>32393751</t>
+  </si>
+  <si>
+    <t>32393752</t>
+  </si>
+  <si>
+    <t>32393753</t>
+  </si>
+  <si>
+    <t>32393754</t>
+  </si>
+  <si>
+    <t>32393755</t>
+  </si>
+  <si>
+    <t>32393756</t>
+  </si>
+  <si>
+    <t>32393757</t>
+  </si>
+  <si>
+    <t>32393758</t>
+  </si>
+  <si>
+    <t>32395699</t>
+  </si>
+  <si>
+    <t>32395700</t>
+  </si>
+  <si>
+    <t>32395701</t>
+  </si>
+  <si>
+    <t>32395702</t>
+  </si>
+  <si>
+    <t>32395703</t>
+  </si>
+  <si>
+    <t>32395704</t>
+  </si>
+  <si>
+    <t>32395705</t>
+  </si>
+  <si>
+    <t>32395706</t>
+  </si>
+  <si>
+    <t>32395707</t>
+  </si>
+  <si>
+    <t>32395708</t>
+  </si>
+  <si>
+    <t>32397358</t>
+  </si>
+  <si>
+    <t>32397364</t>
+  </si>
+  <si>
+    <t>32397373</t>
+  </si>
+  <si>
+    <t>32397381</t>
+  </si>
+  <si>
+    <t>32397382</t>
+  </si>
+  <si>
+    <t>32397389</t>
+  </si>
+  <si>
+    <t>32397396</t>
+  </si>
+  <si>
+    <t>32397397</t>
+  </si>
+  <si>
+    <t>32397404</t>
+  </si>
+  <si>
+    <t>32397405</t>
+  </si>
+  <si>
+    <t>32255134</t>
+  </si>
+  <si>
+    <t>32255135</t>
+  </si>
+  <si>
+    <t>32255136</t>
+  </si>
+  <si>
+    <t>32255137</t>
+  </si>
+  <si>
+    <t>32255138</t>
+  </si>
+  <si>
+    <t>32255139</t>
+  </si>
+  <si>
+    <t>32255140</t>
+  </si>
+  <si>
+    <t>32255141</t>
+  </si>
+  <si>
+    <t>32255142</t>
+  </si>
+  <si>
+    <t>32255143</t>
+  </si>
+  <si>
+    <t>32255216</t>
+  </si>
+  <si>
+    <t>32255217</t>
+  </si>
+  <si>
+    <t>32255218</t>
+  </si>
+  <si>
+    <t>32255219</t>
+  </si>
+  <si>
+    <t>32255220</t>
+  </si>
+  <si>
+    <t>32255221</t>
+  </si>
+  <si>
+    <t>32255222</t>
+  </si>
+  <si>
+    <t>32255223</t>
+  </si>
+  <si>
+    <t>32255224</t>
+  </si>
+  <si>
+    <t>32255225</t>
   </si>
 </sst>
 </file>
@@ -1723,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>434</v>
+        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1731,7 +2121,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>435</v>
+        <v>565</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1739,7 +2129,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>436</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1747,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>437</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1755,7 +2145,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>438</v>
+        <v>568</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1763,7 +2153,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>439</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1771,7 +2161,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>440</v>
+        <v>570</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1779,7 +2169,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>441</v>
+        <v>571</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1787,7 +2177,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>442</v>
+        <v>572</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1795,7 +2185,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>443</v>
+        <v>573</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>

<commit_message>
Changes of Final Config
</commit_message>
<xml_diff>
--- a/FedExCIL/TestFiles/FedExCILTestResult.xlsx
+++ b/FedExCIL/TestFiles/FedExCILTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="604">
   <si>
     <t>FileName</t>
   </si>
@@ -1736,6 +1736,96 @@
   </si>
   <si>
     <t>32255225</t>
+  </si>
+  <si>
+    <t>32255226</t>
+  </si>
+  <si>
+    <t>32255227</t>
+  </si>
+  <si>
+    <t>32255228</t>
+  </si>
+  <si>
+    <t>32255229</t>
+  </si>
+  <si>
+    <t>32255230</t>
+  </si>
+  <si>
+    <t>32255231</t>
+  </si>
+  <si>
+    <t>32255232</t>
+  </si>
+  <si>
+    <t>32255233</t>
+  </si>
+  <si>
+    <t>32255234</t>
+  </si>
+  <si>
+    <t>32255235</t>
+  </si>
+  <si>
+    <t>32255236</t>
+  </si>
+  <si>
+    <t>32255237</t>
+  </si>
+  <si>
+    <t>32255238</t>
+  </si>
+  <si>
+    <t>32255239</t>
+  </si>
+  <si>
+    <t>32255240</t>
+  </si>
+  <si>
+    <t>32255241</t>
+  </si>
+  <si>
+    <t>32255242</t>
+  </si>
+  <si>
+    <t>32255243</t>
+  </si>
+  <si>
+    <t>32255244</t>
+  </si>
+  <si>
+    <t>32255245</t>
+  </si>
+  <si>
+    <t>32255246</t>
+  </si>
+  <si>
+    <t>32255247</t>
+  </si>
+  <si>
+    <t>32255248</t>
+  </si>
+  <si>
+    <t>32255249</t>
+  </si>
+  <si>
+    <t>32255250</t>
+  </si>
+  <si>
+    <t>32255251</t>
+  </si>
+  <si>
+    <t>32255252</t>
+  </si>
+  <si>
+    <t>32255253</t>
+  </si>
+  <si>
+    <t>32255254</t>
+  </si>
+  <si>
+    <t>32255255</t>
   </si>
 </sst>
 </file>
@@ -2113,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>564</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2121,7 +2211,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>565</v>
+        <v>595</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2129,7 +2219,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>566</v>
+        <v>596</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2137,7 +2227,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>567</v>
+        <v>597</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2145,7 +2235,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>568</v>
+        <v>598</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2153,7 +2243,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>569</v>
+        <v>599</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2161,7 +2251,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>570</v>
+        <v>600</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2169,7 +2259,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>571</v>
+        <v>601</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2177,7 +2267,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>572</v>
+        <v>602</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2185,7 +2275,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>573</v>
+        <v>603</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>

<commit_message>
Changes to get fail response
</commit_message>
<xml_diff>
--- a/FedExCIL/TestFiles/FedExCILTestResult.xlsx
+++ b/FedExCIL/TestFiles/FedExCILTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="948">
   <si>
     <t>FileName</t>
   </si>
@@ -1826,6 +1826,1038 @@
   </si>
   <si>
     <t>32255255</t>
+  </si>
+  <si>
+    <t>32255257</t>
+  </si>
+  <si>
+    <t>32255258</t>
+  </si>
+  <si>
+    <t>32255259</t>
+  </si>
+  <si>
+    <t>32255260</t>
+  </si>
+  <si>
+    <t>32255261</t>
+  </si>
+  <si>
+    <t>32255262</t>
+  </si>
+  <si>
+    <t>32255263</t>
+  </si>
+  <si>
+    <t>32255264</t>
+  </si>
+  <si>
+    <t>32255265</t>
+  </si>
+  <si>
+    <t>32255266</t>
+  </si>
+  <si>
+    <t>32255267</t>
+  </si>
+  <si>
+    <t>32255268</t>
+  </si>
+  <si>
+    <t>32255269</t>
+  </si>
+  <si>
+    <t>32255270</t>
+  </si>
+  <si>
+    <t>32255271</t>
+  </si>
+  <si>
+    <t>32255272</t>
+  </si>
+  <si>
+    <t>32255273</t>
+  </si>
+  <si>
+    <t>32255274</t>
+  </si>
+  <si>
+    <t>32255275</t>
+  </si>
+  <si>
+    <t>32255276</t>
+  </si>
+  <si>
+    <t>32255277</t>
+  </si>
+  <si>
+    <t>32255278</t>
+  </si>
+  <si>
+    <t>32255279</t>
+  </si>
+  <si>
+    <t>32255281</t>
+  </si>
+  <si>
+    <t>32255282</t>
+  </si>
+  <si>
+    <t>32255283</t>
+  </si>
+  <si>
+    <t>32255284</t>
+  </si>
+  <si>
+    <t>32255287</t>
+  </si>
+  <si>
+    <t>32255288</t>
+  </si>
+  <si>
+    <t>32255289</t>
+  </si>
+  <si>
+    <t>32255290</t>
+  </si>
+  <si>
+    <t>32255291</t>
+  </si>
+  <si>
+    <t>32255292</t>
+  </si>
+  <si>
+    <t>32255293</t>
+  </si>
+  <si>
+    <t>32255294</t>
+  </si>
+  <si>
+    <t>32255296</t>
+  </si>
+  <si>
+    <t>32255297</t>
+  </si>
+  <si>
+    <t>32255299</t>
+  </si>
+  <si>
+    <t>32255300</t>
+  </si>
+  <si>
+    <t>32255302</t>
+  </si>
+  <si>
+    <t>32255303</t>
+  </si>
+  <si>
+    <t>32255304</t>
+  </si>
+  <si>
+    <t>32255305</t>
+  </si>
+  <si>
+    <t>32255306</t>
+  </si>
+  <si>
+    <t>32255307</t>
+  </si>
+  <si>
+    <t>32255308</t>
+  </si>
+  <si>
+    <t>32255309</t>
+  </si>
+  <si>
+    <t>32255310</t>
+  </si>
+  <si>
+    <t>32255311</t>
+  </si>
+  <si>
+    <t>32255312</t>
+  </si>
+  <si>
+    <t>32255313</t>
+  </si>
+  <si>
+    <t>32255314</t>
+  </si>
+  <si>
+    <t>32402515</t>
+  </si>
+  <si>
+    <t>32402516</t>
+  </si>
+  <si>
+    <t>32402519</t>
+  </si>
+  <si>
+    <t>32402522</t>
+  </si>
+  <si>
+    <t>32402525</t>
+  </si>
+  <si>
+    <t>32402526</t>
+  </si>
+  <si>
+    <t>32402529</t>
+  </si>
+  <si>
+    <t>32402533</t>
+  </si>
+  <si>
+    <t>32402536</t>
+  </si>
+  <si>
+    <t>32402537</t>
+  </si>
+  <si>
+    <t>32402585</t>
+  </si>
+  <si>
+    <t>32255316</t>
+  </si>
+  <si>
+    <t>32403199</t>
+  </si>
+  <si>
+    <t>32403200</t>
+  </si>
+  <si>
+    <t>32403201</t>
+  </si>
+  <si>
+    <t>32403204</t>
+  </si>
+  <si>
+    <t>32403205</t>
+  </si>
+  <si>
+    <t>32403206</t>
+  </si>
+  <si>
+    <t>32403207</t>
+  </si>
+  <si>
+    <t>32403208</t>
+  </si>
+  <si>
+    <t>32403209</t>
+  </si>
+  <si>
+    <t>32403210</t>
+  </si>
+  <si>
+    <t>32255318</t>
+  </si>
+  <si>
+    <t>32255319</t>
+  </si>
+  <si>
+    <t>32255320</t>
+  </si>
+  <si>
+    <t>32255321</t>
+  </si>
+  <si>
+    <t>32255322</t>
+  </si>
+  <si>
+    <t>32255323</t>
+  </si>
+  <si>
+    <t>32255324</t>
+  </si>
+  <si>
+    <t>32255325</t>
+  </si>
+  <si>
+    <t>32255326</t>
+  </si>
+  <si>
+    <t>32255327</t>
+  </si>
+  <si>
+    <t>32404718</t>
+  </si>
+  <si>
+    <t>32404719</t>
+  </si>
+  <si>
+    <t>32404720</t>
+  </si>
+  <si>
+    <t>32404721</t>
+  </si>
+  <si>
+    <t>32404722</t>
+  </si>
+  <si>
+    <t>32404729</t>
+  </si>
+  <si>
+    <t>32404730</t>
+  </si>
+  <si>
+    <t>32404731</t>
+  </si>
+  <si>
+    <t>32404732</t>
+  </si>
+  <si>
+    <t>32404733</t>
+  </si>
+  <si>
+    <t>32406336</t>
+  </si>
+  <si>
+    <t>32406337</t>
+  </si>
+  <si>
+    <t>32406339</t>
+  </si>
+  <si>
+    <t>32406340</t>
+  </si>
+  <si>
+    <t>32406341</t>
+  </si>
+  <si>
+    <t>32406342</t>
+  </si>
+  <si>
+    <t>32406343</t>
+  </si>
+  <si>
+    <t>32406344</t>
+  </si>
+  <si>
+    <t>32406345</t>
+  </si>
+  <si>
+    <t>32406346</t>
+  </si>
+  <si>
+    <t>32408017</t>
+  </si>
+  <si>
+    <t>32408018</t>
+  </si>
+  <si>
+    <t>32408019</t>
+  </si>
+  <si>
+    <t>32408020</t>
+  </si>
+  <si>
+    <t>32408021</t>
+  </si>
+  <si>
+    <t>32408022</t>
+  </si>
+  <si>
+    <t>32408023</t>
+  </si>
+  <si>
+    <t>32408024</t>
+  </si>
+  <si>
+    <t>32408025</t>
+  </si>
+  <si>
+    <t>32408026</t>
+  </si>
+  <si>
+    <t>32255339</t>
+  </si>
+  <si>
+    <t>32255340</t>
+  </si>
+  <si>
+    <t>32255341</t>
+  </si>
+  <si>
+    <t>32255342</t>
+  </si>
+  <si>
+    <t>32255343</t>
+  </si>
+  <si>
+    <t>32255344</t>
+  </si>
+  <si>
+    <t>32255345</t>
+  </si>
+  <si>
+    <t>32255346</t>
+  </si>
+  <si>
+    <t>32255348</t>
+  </si>
+  <si>
+    <t>32255349</t>
+  </si>
+  <si>
+    <t>32411154</t>
+  </si>
+  <si>
+    <t>32411155</t>
+  </si>
+  <si>
+    <t>32411156</t>
+  </si>
+  <si>
+    <t>32411157</t>
+  </si>
+  <si>
+    <t>32411158</t>
+  </si>
+  <si>
+    <t>32411159</t>
+  </si>
+  <si>
+    <t>32411160</t>
+  </si>
+  <si>
+    <t>32411161</t>
+  </si>
+  <si>
+    <t>32411162</t>
+  </si>
+  <si>
+    <t>32411163</t>
+  </si>
+  <si>
+    <t>32413040</t>
+  </si>
+  <si>
+    <t>32413041</t>
+  </si>
+  <si>
+    <t>32413042</t>
+  </si>
+  <si>
+    <t>32413043</t>
+  </si>
+  <si>
+    <t>32413044</t>
+  </si>
+  <si>
+    <t>32413045</t>
+  </si>
+  <si>
+    <t>32413046</t>
+  </si>
+  <si>
+    <t>32413047</t>
+  </si>
+  <si>
+    <t>32413048</t>
+  </si>
+  <si>
+    <t>32413049</t>
+  </si>
+  <si>
+    <t>32415082</t>
+  </si>
+  <si>
+    <t>32415083</t>
+  </si>
+  <si>
+    <t>32415085</t>
+  </si>
+  <si>
+    <t>32415093</t>
+  </si>
+  <si>
+    <t>32415094</t>
+  </si>
+  <si>
+    <t>32415102</t>
+  </si>
+  <si>
+    <t>32415103</t>
+  </si>
+  <si>
+    <t>32415112</t>
+  </si>
+  <si>
+    <t>32415113</t>
+  </si>
+  <si>
+    <t>32415121</t>
+  </si>
+  <si>
+    <t>32416901</t>
+  </si>
+  <si>
+    <t>32416902</t>
+  </si>
+  <si>
+    <t>32416906</t>
+  </si>
+  <si>
+    <t>32416907</t>
+  </si>
+  <si>
+    <t>32416908</t>
+  </si>
+  <si>
+    <t>32416909</t>
+  </si>
+  <si>
+    <t>32416910</t>
+  </si>
+  <si>
+    <t>32416911</t>
+  </si>
+  <si>
+    <t>32416912</t>
+  </si>
+  <si>
+    <t>32416913</t>
+  </si>
+  <si>
+    <t>32255446</t>
+  </si>
+  <si>
+    <t>32255447</t>
+  </si>
+  <si>
+    <t>32255448</t>
+  </si>
+  <si>
+    <t>32255449</t>
+  </si>
+  <si>
+    <t>32255450</t>
+  </si>
+  <si>
+    <t>32255451</t>
+  </si>
+  <si>
+    <t>32255453</t>
+  </si>
+  <si>
+    <t>32255454</t>
+  </si>
+  <si>
+    <t>32255456</t>
+  </si>
+  <si>
+    <t>32255457</t>
+  </si>
+  <si>
+    <t>32418686</t>
+  </si>
+  <si>
+    <t>32418687</t>
+  </si>
+  <si>
+    <t>32418688</t>
+  </si>
+  <si>
+    <t>32418692</t>
+  </si>
+  <si>
+    <t>32418693</t>
+  </si>
+  <si>
+    <t>32418694</t>
+  </si>
+  <si>
+    <t>32418695</t>
+  </si>
+  <si>
+    <t>32418696</t>
+  </si>
+  <si>
+    <t>32418697</t>
+  </si>
+  <si>
+    <t>32418699</t>
+  </si>
+  <si>
+    <t>32255510</t>
+  </si>
+  <si>
+    <t>32255511</t>
+  </si>
+  <si>
+    <t>32255512</t>
+  </si>
+  <si>
+    <t>32255513</t>
+  </si>
+  <si>
+    <t>32255514</t>
+  </si>
+  <si>
+    <t>32255515</t>
+  </si>
+  <si>
+    <t>32255516</t>
+  </si>
+  <si>
+    <t>32255517</t>
+  </si>
+  <si>
+    <t>32255518</t>
+  </si>
+  <si>
+    <t>32255519</t>
+  </si>
+  <si>
+    <t>32422881</t>
+  </si>
+  <si>
+    <t>32422882</t>
+  </si>
+  <si>
+    <t>32422883</t>
+  </si>
+  <si>
+    <t>32422884</t>
+  </si>
+  <si>
+    <t>32422885</t>
+  </si>
+  <si>
+    <t>32422886</t>
+  </si>
+  <si>
+    <t>32422887</t>
+  </si>
+  <si>
+    <t>32422888</t>
+  </si>
+  <si>
+    <t>32422889</t>
+  </si>
+  <si>
+    <t>32422890</t>
+  </si>
+  <si>
+    <t>32422962</t>
+  </si>
+  <si>
+    <t>32422963</t>
+  </si>
+  <si>
+    <t>32422964</t>
+  </si>
+  <si>
+    <t>32422965</t>
+  </si>
+  <si>
+    <t>32422966</t>
+  </si>
+  <si>
+    <t>32422967</t>
+  </si>
+  <si>
+    <t>32422968</t>
+  </si>
+  <si>
+    <t>32422969</t>
+  </si>
+  <si>
+    <t>32422970</t>
+  </si>
+  <si>
+    <t>32422971</t>
+  </si>
+  <si>
+    <t>32424968</t>
+  </si>
+  <si>
+    <t>32424976</t>
+  </si>
+  <si>
+    <t>32424978</t>
+  </si>
+  <si>
+    <t>32424981</t>
+  </si>
+  <si>
+    <t>32424989</t>
+  </si>
+  <si>
+    <t>32424991</t>
+  </si>
+  <si>
+    <t>32424992</t>
+  </si>
+  <si>
+    <t>32424993</t>
+  </si>
+  <si>
+    <t>32424994</t>
+  </si>
+  <si>
+    <t>32424995</t>
+  </si>
+  <si>
+    <t>32426664</t>
+  </si>
+  <si>
+    <t>32426665</t>
+  </si>
+  <si>
+    <t>32426666</t>
+  </si>
+  <si>
+    <t>32426667</t>
+  </si>
+  <si>
+    <t>32426668</t>
+  </si>
+  <si>
+    <t>32426669</t>
+  </si>
+  <si>
+    <t>32426670</t>
+  </si>
+  <si>
+    <t>32426671</t>
+  </si>
+  <si>
+    <t>32426672</t>
+  </si>
+  <si>
+    <t>32426673</t>
+  </si>
+  <si>
+    <t>32428451</t>
+  </si>
+  <si>
+    <t>32428452</t>
+  </si>
+  <si>
+    <t>32428453</t>
+  </si>
+  <si>
+    <t>32428454</t>
+  </si>
+  <si>
+    <t>32428455</t>
+  </si>
+  <si>
+    <t>32428456</t>
+  </si>
+  <si>
+    <t>32428457</t>
+  </si>
+  <si>
+    <t>32428458</t>
+  </si>
+  <si>
+    <t>32428461</t>
+  </si>
+  <si>
+    <t>32428462</t>
+  </si>
+  <si>
+    <t>32255538</t>
+  </si>
+  <si>
+    <t>32255539</t>
+  </si>
+  <si>
+    <t>32255540</t>
+  </si>
+  <si>
+    <t>32255541</t>
+  </si>
+  <si>
+    <t>32255542</t>
+  </si>
+  <si>
+    <t>32255543</t>
+  </si>
+  <si>
+    <t>32255544</t>
+  </si>
+  <si>
+    <t>32255545</t>
+  </si>
+  <si>
+    <t>32255546</t>
+  </si>
+  <si>
+    <t>32255547</t>
+  </si>
+  <si>
+    <t>32431936</t>
+  </si>
+  <si>
+    <t>32431937</t>
+  </si>
+  <si>
+    <t>32431938</t>
+  </si>
+  <si>
+    <t>32431939</t>
+  </si>
+  <si>
+    <t>32431940</t>
+  </si>
+  <si>
+    <t>32431941</t>
+  </si>
+  <si>
+    <t>32431942</t>
+  </si>
+  <si>
+    <t>32431943</t>
+  </si>
+  <si>
+    <t>32431944</t>
+  </si>
+  <si>
+    <t>32431945</t>
+  </si>
+  <si>
+    <t>32434184</t>
+  </si>
+  <si>
+    <t>32434185</t>
+  </si>
+  <si>
+    <t>32434186</t>
+  </si>
+  <si>
+    <t>32434187</t>
+  </si>
+  <si>
+    <t>32434188</t>
+  </si>
+  <si>
+    <t>32434189</t>
+  </si>
+  <si>
+    <t>32434190</t>
+  </si>
+  <si>
+    <t>32434191</t>
+  </si>
+  <si>
+    <t>32434192</t>
+  </si>
+  <si>
+    <t>32434193</t>
+  </si>
+  <si>
+    <t>32436307</t>
+  </si>
+  <si>
+    <t>32436308</t>
+  </si>
+  <si>
+    <t>32436309</t>
+  </si>
+  <si>
+    <t>32436310</t>
+  </si>
+  <si>
+    <t>32436311</t>
+  </si>
+  <si>
+    <t>32436312</t>
+  </si>
+  <si>
+    <t>32436313</t>
+  </si>
+  <si>
+    <t>32436314</t>
+  </si>
+  <si>
+    <t>32436315</t>
+  </si>
+  <si>
+    <t>32436323</t>
+  </si>
+  <si>
+    <t>32438284</t>
+  </si>
+  <si>
+    <t>32438285</t>
+  </si>
+  <si>
+    <t>32438286</t>
+  </si>
+  <si>
+    <t>32438287</t>
+  </si>
+  <si>
+    <t>32438288</t>
+  </si>
+  <si>
+    <t>32438289</t>
+  </si>
+  <si>
+    <t>32438290</t>
+  </si>
+  <si>
+    <t>32438292</t>
+  </si>
+  <si>
+    <t>32438293</t>
+  </si>
+  <si>
+    <t>32438294</t>
+  </si>
+  <si>
+    <t>32440205</t>
+  </si>
+  <si>
+    <t>32440206</t>
+  </si>
+  <si>
+    <t>32440208</t>
+  </si>
+  <si>
+    <t>32440209</t>
+  </si>
+  <si>
+    <t>32440211</t>
+  </si>
+  <si>
+    <t>32440212</t>
+  </si>
+  <si>
+    <t>32440213</t>
+  </si>
+  <si>
+    <t>32440214</t>
+  </si>
+  <si>
+    <t>32440215</t>
+  </si>
+  <si>
+    <t>32440216</t>
+  </si>
+  <si>
+    <t>32255669</t>
+  </si>
+  <si>
+    <t>32255670</t>
+  </si>
+  <si>
+    <t>32255671</t>
+  </si>
+  <si>
+    <t>32255672</t>
+  </si>
+  <si>
+    <t>32255673</t>
+  </si>
+  <si>
+    <t>32255674</t>
+  </si>
+  <si>
+    <t>32255675</t>
+  </si>
+  <si>
+    <t>32255676</t>
+  </si>
+  <si>
+    <t>32255677</t>
+  </si>
+  <si>
+    <t>32255678</t>
+  </si>
+  <si>
+    <t>32443668</t>
+  </si>
+  <si>
+    <t>32443671</t>
+  </si>
+  <si>
+    <t>32443680</t>
+  </si>
+  <si>
+    <t>32443687</t>
+  </si>
+  <si>
+    <t>32443688</t>
+  </si>
+  <si>
+    <t>32443689</t>
+  </si>
+  <si>
+    <t>32443690</t>
+  </si>
+  <si>
+    <t>32443691</t>
+  </si>
+  <si>
+    <t>32443692</t>
+  </si>
+  <si>
+    <t>32443693</t>
+  </si>
+  <si>
+    <t>32445567</t>
+  </si>
+  <si>
+    <t>32445568</t>
+  </si>
+  <si>
+    <t>32445569</t>
+  </si>
+  <si>
+    <t>32445570</t>
+  </si>
+  <si>
+    <t>32445571</t>
+  </si>
+  <si>
+    <t>32445572</t>
+  </si>
+  <si>
+    <t>32445573</t>
+  </si>
+  <si>
+    <t>32445574</t>
+  </si>
+  <si>
+    <t>32445575</t>
+  </si>
+  <si>
+    <t>32445576</t>
+  </si>
+  <si>
+    <t>32447785</t>
+  </si>
+  <si>
+    <t>32447786</t>
+  </si>
+  <si>
+    <t>32447787</t>
+  </si>
+  <si>
+    <t>32447788</t>
+  </si>
+  <si>
+    <t>32447789</t>
+  </si>
+  <si>
+    <t>32447790</t>
+  </si>
+  <si>
+    <t>32447791</t>
+  </si>
+  <si>
+    <t>32447792</t>
+  </si>
+  <si>
+    <t>32447793</t>
+  </si>
+  <si>
+    <t>32447794</t>
   </si>
 </sst>
 </file>
@@ -2203,7 +3235,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>594</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2211,7 +3243,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>595</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2219,7 +3251,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>596</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2227,7 +3259,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>597</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2235,7 +3267,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>598</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2243,7 +3275,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>599</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2251,7 +3283,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>600</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2259,7 +3291,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>601</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2267,7 +3299,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>602</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2275,7 +3307,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>603</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>